<commit_message>
Updated mapping for treatment instructions
</commit_message>
<xml_diff>
--- a/Mappings/TreatmentInstructions.xlsx
+++ b/Mappings/TreatmentInstructions.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="156">
   <si>
     <t>Onderwerp</t>
   </si>
@@ -470,15 +470,9 @@
     <t>Consent.policyRule</t>
   </si>
   <si>
-    <t>Nu een uri met: -http://hl7.org/fhir/ConsentPolicy/opt-out of http://hl7.org/fhir/ConsentPolicy/opt-in</t>
-  </si>
-  <si>
     <t>Consent.noteExtension</t>
   </si>
   <si>
-    <t>Consent.Data.Reference(Consent)</t>
-  </si>
-  <si>
     <t>Is Coding in FHIR, should be CodeableConcept so we can add text</t>
   </si>
   <si>
@@ -492,6 +486,24 @@
   </si>
   <si>
     <t>Consent.verificationExtension</t>
+  </si>
+  <si>
+    <t>Consent.consentingParty</t>
+  </si>
+  <si>
+    <t>Should this be consent.consentingParty? Then we only need an extension for dateTime. However, consentingParty in FHIR is a reference to a person, instead of just a code that indicates the role of the person.</t>
+  </si>
+  <si>
+    <t>gForge? Renaming purpose to context?</t>
+  </si>
+  <si>
+    <t>Nu een uri met: -http://hl7.org/fhir/ConsentPolicy/opt-out of http://hl7.org/fhir/ConsentPolicy/opt-in. Zulip. Action misschien?</t>
+  </si>
+  <si>
+    <t>gForge?</t>
+  </si>
+  <si>
+    <t>Consent.Source.Reference(Consent)</t>
   </si>
 </sst>
 </file>
@@ -530,7 +542,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +570,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -688,25 +706,34 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1179,10 +1206,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -1411,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1449,7 @@
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="10" width="5.7109375" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" customWidth="1"/>
     <col min="13" max="14" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1447,10 +1474,10 @@
       <c r="K2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="18" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1473,7 +1500,7 @@
       <c r="K3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="19" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1496,7 +1523,10 @@
       <c r="K4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="M4" s="26" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1542,6 +1572,9 @@
       </c>
       <c r="K6" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,11 +1620,14 @@
       <c r="K8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="M8" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" s="15" t="s">
         <v>83</v>
@@ -1612,11 +1648,11 @@
       <c r="K9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="M9" s="22" t="s">
-        <v>144</v>
+      <c r="M9" s="25" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="45" x14ac:dyDescent="0.25">
@@ -1640,11 +1676,11 @@
       <c r="K10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="M10" s="22" t="s">
-        <v>147</v>
+      <c r="L10" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1668,8 +1704,8 @@
       <c r="K11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="23" t="s">
-        <v>149</v>
+      <c r="L11" s="21" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1693,8 +1729,8 @@
       <c r="K12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L12" s="23" t="s">
-        <v>150</v>
+      <c r="L12" s="21" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1718,8 +1754,11 @@
       <c r="K13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L13" s="23" t="s">
-        <v>145</v>
+      <c r="L13" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1741,8 +1780,8 @@
       <c r="K14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="23" t="s">
-        <v>146</v>
+      <c r="L14" s="21" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1766,15 +1805,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
@@ -1903,15 +1942,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
@@ -2006,15 +2045,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">

</xml_diff>